<commit_message>
just need to do reaction time and check
</commit_message>
<xml_diff>
--- a/tablet_exp/images/Major.xlsx
+++ b/tablet_exp/images/Major.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14820" yWindow="0" windowWidth="10780" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="15260" yWindow="0" windowWidth="10780" windowHeight="14720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>Psych Course</t>
   </si>
@@ -124,6 +124,51 @@
   </si>
   <si>
     <t>Classics GPA</t>
+  </si>
+  <si>
+    <t>Intro 1</t>
+  </si>
+  <si>
+    <t>Intro 2</t>
+  </si>
+  <si>
+    <t>Intro 3</t>
+  </si>
+  <si>
+    <t>Stats I</t>
+  </si>
+  <si>
+    <t>Stats II</t>
+  </si>
+  <si>
+    <t>Research Methods</t>
+  </si>
+  <si>
+    <t>3 N</t>
+  </si>
+  <si>
+    <t>Cog Psych</t>
+  </si>
+  <si>
+    <t>Dev Pysch</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>Evolutionary</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Abnormal</t>
+  </si>
+  <si>
+    <t>Planets</t>
+  </si>
+  <si>
+    <t>Visual Cognition</t>
   </si>
 </sst>
 </file>
@@ -512,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -966,7 +1011,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="1:8">
       <c r="E17" t="s">
         <v>32</v>
       </c>
@@ -981,7 +1026,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="1:8">
       <c r="B19" t="s">
         <v>33</v>
       </c>
@@ -995,6 +1040,282 @@
       <c r="G19">
         <f>((SUM(H2:H17))/(SUM(G2:G17)))</f>
         <v>3.9773584905660377</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <f>(D20*C20)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21:E34" si="2">(D21*C21)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22">
+        <v>3.7</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>11.100000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>200</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>200</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>300</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>300</v>
+      </c>
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>300</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="D36">
+        <f>(SUM(E20:E34))/(SUM(D20:D34))</f>
+        <v>3.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>